<commit_message>
export data to Excel and handle pagination
</commit_message>
<xml_diff>
--- a/selectors.xlsx
+++ b/selectors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>//button[@aria-current='page']</t>
+  </si>
+  <si>
+    <t>suivant</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/div/section/div[1]/div[1]/div[2]/div[2]/div[2]/nav/div[3]/button</t>
   </si>
 </sst>
 </file>
@@ -147,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -162,9 +168,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -472,7 +475,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -481,10 +484,10 @@
     <col min="1" max="1" style="6" width="36.57642857142857" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="71.57642857142856" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="66.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,6 +606,16 @@
         <v>5</v>
       </c>
       <c r="D10" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor: split scraper logic into feature-based modules.
</commit_message>
<xml_diff>
--- a/selectors.xlsx
+++ b/selectors.xlsx
@@ -43,13 +43,13 @@
     <t>taille_label</t>
   </si>
   <si>
-    <t>/html/body/div[3]/div/section/div[1]/div[1]/div[1]/section[1]/section[5]/label</t>
+    <t>/html/body/div[3]/div/section/div[1]/div[1]/div[1]/section[1]/section[3]/label</t>
   </si>
   <si>
     <t>douze_pouces</t>
   </si>
   <si>
-    <t>/html/body/div[3]/div/section/div[1]/div[1]/div[1]/section[1]/section[5]/div/div/label[1]</t>
+    <t>/html/body/div[3]/div/section/div[1]/div[1]/div[1]/section[1]/section[3]/div/div/label[1]</t>
   </si>
   <si>
     <t>category</t>
@@ -61,7 +61,7 @@
     <t>number_products</t>
   </si>
   <si>
-    <t>/html/body/div[3]/div/section/div[1]/div[1]/div[1]/section[1]/section[5]/div/div/label[1]/span[2]/span</t>
+    <t>/html/body/div[3]/div/section/div[1]/div[1]/div[1]/section[1]/section[3]/div/div/label[1]/span[2]/span</t>
   </si>
   <si>
     <t>number_filters</t>
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -168,6 +168,9 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -483,11 +486,11 @@
   <cols>
     <col min="1" max="1" style="6" width="36.57642857142857" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="71.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="66.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="66.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +610,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>